<commit_message>
Nifty 50 Return of Change Tracker - added readme.md
</commit_message>
<xml_diff>
--- a/Nifty50ReturnofChangeTracker/code/output/nifty_roc_summary.xlsx
+++ b/Nifty50ReturnofChangeTracker/code/output/nifty_roc_summary.xlsx
@@ -446,7 +446,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>60-Day ROC (%)</t>
+          <t>30-Day ROC (%)</t>
         </is>
       </c>
     </row>
@@ -460,202 +460,202 @@
         <v>318.3999938964844</v>
       </c>
       <c r="C2" t="n">
-        <v>39.02715394140404</v>
+        <v>22.06248282399144</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>JIOFIN.NS</t>
+          <t>HEROMOTOCO.NS</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>327.3999938964844</v>
+        <v>4708.10009765625</v>
       </c>
       <c r="C3" t="n">
-        <v>19.24968437564401</v>
+        <v>9.221453881006681</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>APOLLOHOSP.NS</t>
+          <t>HINDUNILVR.NS</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>7821.5</v>
+        <v>2480.60009765625</v>
       </c>
       <c r="C4" t="n">
-        <v>12.46674814868072</v>
+        <v>7.227466169731667</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HEROMOTOCO.NS</t>
+          <t>ASIANPAINT.NS</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4708.10009765625</v>
+        <v>2528.699951171875</v>
       </c>
       <c r="C5" t="n">
-        <v>10.0975215183797</v>
+        <v>4.02320345374283</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ASIANPAINT.NS</t>
+          <t>CIPLA.NS</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2528.699951171875</v>
+        <v>1564</v>
       </c>
       <c r="C6" t="n">
-        <v>9.981732988600079</v>
+        <v>3.66541065936743</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>M&amp;M.NS</t>
+          <t>APOLLOHOSP.NS</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3265.39990234375</v>
+        <v>7821.5</v>
       </c>
       <c r="C7" t="n">
-        <v>8.618562661987905</v>
+        <v>3.390614672835435</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>HINDALCO.NS</t>
+          <t>M&amp;M.NS</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>695.25</v>
+        <v>3265.39990234375</v>
       </c>
       <c r="C8" t="n">
-        <v>7.035642070029136</v>
+        <v>2.866683555931693</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>EICHERMOT.NS</t>
+          <t>LT.NS</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>5764</v>
+        <v>3677</v>
       </c>
       <c r="C9" t="n">
-        <v>6.998329311304996</v>
+        <v>2.62636691565663</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CIPLA.NS</t>
+          <t>SBIN.NS</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1564</v>
+        <v>826.5499877929688</v>
       </c>
       <c r="C10" t="n">
-        <v>6.503234593122231</v>
+        <v>2.409864055925781</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>HINDUNILVR.NS</t>
+          <t>SBILIFE.NS</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2480.60009765625</v>
+        <v>1840.599975585938</v>
       </c>
       <c r="C11" t="n">
-        <v>6.431550591014745</v>
+        <v>1.679373839027143</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ULTRACEMCO.NS</t>
+          <t>MARUTI.NS</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>12317</v>
+        <v>12936</v>
       </c>
       <c r="C12" t="n">
-        <v>5.453767123287667</v>
+        <v>1.442910915934759</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>SBIN.NS</t>
+          <t>NTPC.NS</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>826.5499877929688</v>
+        <v>339.3500061035156</v>
       </c>
       <c r="C13" t="n">
-        <v>5.259469951349094</v>
+        <v>1.419605473208052</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>SBILIFE.NS</t>
+          <t>EICHERMOT.NS</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1840.599975585938</v>
+        <v>5764</v>
       </c>
       <c r="C14" t="n">
-        <v>4.621151850246719</v>
+        <v>0.8397480755773179</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>HDFCLIFE.NS</t>
+          <t>JIOFIN.NS</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>788.75</v>
+        <v>327.3999938964844</v>
       </c>
       <c r="C15" t="n">
-        <v>4.352718856484494</v>
+        <v>0.7229676024514742</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>JSWSTEEL.NS</t>
+          <t>HDFCLIFE.NS</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1045.5</v>
+        <v>788.75</v>
       </c>
       <c r="C16" t="n">
-        <v>3.967782953735033</v>
+        <v>0.3690302862070061</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>MARUTI.NS</t>
+          <t>HINDALCO.NS</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>12936</v>
+        <v>695.25</v>
       </c>
       <c r="C17" t="n">
-        <v>3.945359582161512</v>
+        <v>0.3463988595846956</v>
       </c>
     </row>
     <row r="18">
@@ -668,215 +668,215 @@
         <v>1991.099975585938</v>
       </c>
       <c r="C18" t="n">
-        <v>3.708523895331717</v>
+        <v>0.2012983769888343</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>LT.NS</t>
+          <t>ICICIBANK.NS</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>3677</v>
+        <v>1427.300048828125</v>
       </c>
       <c r="C19" t="n">
-        <v>3.536636287379524</v>
+        <v>0.09818531384329088</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>GRASIM.NS</t>
+          <t>JSWSTEEL.NS</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>2764.89990234375</v>
+        <v>1045.5</v>
       </c>
       <c r="C20" t="n">
-        <v>3.376198362014171</v>
+        <v>-0.05735356083929055</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>DRREDDY.NS</t>
+          <t>ITC.NS</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1260.400024414062</v>
+        <v>411.4500122070312</v>
       </c>
       <c r="C21" t="n">
-        <v>3.1255174904532</v>
+        <v>-0.459657401337632</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>BHARTIARTL.NS</t>
+          <t>COALINDIA.NS</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1873.800048828125</v>
+        <v>384.4500122070312</v>
       </c>
       <c r="C22" t="n">
-        <v>2.315170025599844</v>
+        <v>-0.5175313589920516</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>TRENT.NS</t>
+          <t>ULTRACEMCO.NS</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>5370.5</v>
+        <v>12317</v>
       </c>
       <c r="C23" t="n">
-        <v>0.5335080494196953</v>
+        <v>-0.6533311824487797</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>BEL.NS</t>
+          <t>POWERGRID.NS</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>384.8999938964844</v>
+        <v>288.7000122070312</v>
       </c>
       <c r="C24" t="n">
-        <v>0.3912363129575214</v>
+        <v>-1.702417361997066</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>WIPRO.NS</t>
+          <t>GRASIM.NS</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>246.8099975585938</v>
+        <v>2764.89990234375</v>
       </c>
       <c r="C25" t="n">
-        <v>0.3537428269298148</v>
+        <v>-1.870393011284222</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>NTPC.NS</t>
+          <t>BAJAJ-AUTO.NS</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>339.3500061035156</v>
+        <v>8213.5</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.600465093619873</v>
+        <v>-2.016104980614375</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>POWERGRID.NS</t>
+          <t>SUNPHARMA.NS</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>288.7000122070312</v>
+        <v>1641.400024414062</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.7562673549714738</v>
+        <v>-2.28016478366222</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>ICICIBANK.NS</t>
+          <t>DRREDDY.NS</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>1427.300048828125</v>
+        <v>1260.400024414062</v>
       </c>
       <c r="C28" t="n">
-        <v>-1.026276056332309</v>
+        <v>-2.392939150130502</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>TITAN.NS</t>
+          <t>BAJAJFINSV.NS</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>3489.39990234375</v>
+        <v>1925.099975585938</v>
       </c>
       <c r="C29" t="n">
-        <v>-1.457218233726354</v>
+        <v>-2.807087239692307</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>INDUSINDBK.NS</t>
+          <t>ONGC.NS</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>769.75</v>
+        <v>236.9400024414062</v>
       </c>
       <c r="C30" t="n">
-        <v>-1.942675159235674</v>
+        <v>-2.913337644516922</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>ONGC.NS</t>
+          <t>TATACONSUM.NS</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>236.9400024414062</v>
+        <v>1051.199951171875</v>
       </c>
       <c r="C31" t="n">
-        <v>-1.957212630188565</v>
+        <v>-3.506523993583854</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>RELIANCE.NS</t>
+          <t>TATAMOTORS.NS</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>1373.800048828125</v>
+        <v>664.5999755859375</v>
       </c>
       <c r="C32" t="n">
-        <v>-2.525895769069375</v>
+        <v>-3.736971019087276</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>ITC.NS</t>
+          <t>TITAN.NS</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>411.4500122070312</v>
+        <v>3489.39990234375</v>
       </c>
       <c r="C33" t="n">
-        <v>-3.438158574662242</v>
+        <v>-5.145840958510961</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>COALINDIA.NS</t>
+          <t>BAJFINANCE.NS</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>384.4500122070312</v>
+        <v>861.4500122070312</v>
       </c>
       <c r="C34" t="n">
-        <v>-3.610378256518587</v>
+        <v>-5.350767554874636</v>
       </c>
     </row>
     <row r="35">
@@ -889,215 +889,215 @@
         <v>155.3000030517578</v>
       </c>
       <c r="C35" t="n">
-        <v>-3.713801527506166</v>
+        <v>-6.395033678595885</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>BAJAJFINSV.NS</t>
+          <t>KOTAKBANK.NS</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>1925.099975585938</v>
+        <v>1978.199951171875</v>
       </c>
       <c r="C36" t="n">
-        <v>-3.793104668368941</v>
+        <v>-6.978281748784287</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>KOTAKBANK.NS</t>
+          <t>BHARTIARTL.NS</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>1978.199951171875</v>
+        <v>1873.800048828125</v>
       </c>
       <c r="C37" t="n">
-        <v>-4.240492573612986</v>
+        <v>-7.205467066889792</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>SUNPHARMA.NS</t>
+          <t>WIPRO.NS</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>1641.400024414062</v>
+        <v>246.8099975585938</v>
       </c>
       <c r="C38" t="n">
-        <v>-4.497581250590398</v>
+        <v>-7.579101726103099</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>TECHM.NS</t>
+          <t>SHRIRAMFIN.NS</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>1486.699951171875</v>
+        <v>616.4500122070312</v>
       </c>
       <c r="C39" t="n">
-        <v>-5.039603068755383</v>
+        <v>-8.728162581600852</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>SHRIRAMFIN.NS</t>
+          <t>NESTLEIND.NS</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>616.4500122070312</v>
+        <v>1089.400024414062</v>
       </c>
       <c r="C40" t="n">
-        <v>-5.125046216693918</v>
+        <v>-8.775743681363558</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>ADANIPORTS.NS</t>
+          <t>AXISBANK.NS</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>1300.300048828125</v>
+        <v>1068.199951171875</v>
       </c>
       <c r="C41" t="n">
-        <v>-5.184481137537922</v>
+        <v>-8.786613146548694</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>BAJFINANCE.NS</t>
+          <t>ADANIPORTS.NS</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>861.4500122070312</v>
+        <v>1300.300048828125</v>
       </c>
       <c r="C42" t="n">
-        <v>-5.739141132057524</v>
+        <v>-9.139817552177576</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>BAJAJ-AUTO.NS</t>
+          <t>RELIANCE.NS</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>8213.5</v>
+        <v>1373.800048828125</v>
       </c>
       <c r="C43" t="n">
-        <v>-5.954084845709051</v>
+        <v>-9.487415691624246</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>INFY.NS</t>
+          <t>BEL.NS</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>1447.699951171875</v>
+        <v>384.8999938964844</v>
       </c>
       <c r="C44" t="n">
-        <v>-6.449114625403873</v>
+        <v>-9.700881197305723</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>TATACONSUM.NS</t>
+          <t>INFY.NS</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>1051.199951171875</v>
+        <v>1447.699951171875</v>
       </c>
       <c r="C45" t="n">
-        <v>-6.700985468355869</v>
+        <v>-10.56403318454434</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>TATAMOTORS.NS</t>
+          <t>INDUSINDBK.NS</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>664.5999755859375</v>
+        <v>769.75</v>
       </c>
       <c r="C46" t="n">
-        <v>-7.366371973221608</v>
+        <v>-10.74327710936829</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>NESTLEIND.NS</t>
+          <t>TECHM.NS</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>1089.400024414062</v>
+        <v>1486.699951171875</v>
       </c>
       <c r="C47" t="n">
-        <v>-7.744417416488281</v>
+        <v>-11.07722175595357</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>ADANIENT.NS</t>
+          <t>TCS.NS</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>2281.60009765625</v>
+        <v>3022.300048828125</v>
       </c>
       <c r="C48" t="n">
-        <v>-8.281073802581362</v>
+        <v>-11.12973402039401</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>HCLTECH.NS</t>
+          <t>ADANIENT.NS</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>1489.800048828125</v>
+        <v>2281.60009765625</v>
       </c>
       <c r="C49" t="n">
-        <v>-8.769133568394061</v>
+        <v>-12.62254364579414</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>AXISBANK.NS</t>
+          <t>HCLTECH.NS</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>1068.199951171875</v>
+        <v>1489.800048828125</v>
       </c>
       <c r="C50" t="n">
-        <v>-10.12200663257257</v>
+        <v>-12.97388705055696</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>TCS.NS</t>
+          <t>TRENT.NS</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>3022.300048828125</v>
+        <v>5370.5</v>
       </c>
       <c r="C51" t="n">
-        <v>-13.0773641406924</v>
+        <v>-13.25310935228558</v>
       </c>
     </row>
   </sheetData>

</xml_diff>